<commit_message>
Primeiro commit: projeto inicial
</commit_message>
<xml_diff>
--- a/Customer bulk email data.xlsx
+++ b/Customer bulk email data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F53F7B-E3E1-4FAC-8B68-CE8EB21B222E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -28,13 +29,13 @@
     <t>Hi {customer_name}, *Offer*: All Surya products having *5% discount* until the end of July for first 50 lucky customers. Visit near by Prestige Group Congo store to get offer.</t>
   </si>
   <si>
-    <t>Mr. Ramesh Kumar</t>
+    <t>Ayres Costa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -64,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -79,7 +80,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,28 +108,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Contact"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Contact"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D1:D2" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="D1:D2" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <tableColumns count="1">
-    <tableColumn id="1" name="Message" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Message" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -167,9 +167,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,7 +204,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,7 +239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,11 +412,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,25 +442,12 @@
         <v>4</v>
       </c>
       <c r="B2" s="5">
-        <v>9155456554</v>
+        <v>5397025835</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5" s="1"/>
-      <c r="D5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>